<commit_message>
Chore : Unity Excel Impoty 패키지 재설치
</commit_message>
<xml_diff>
--- a/Assets/Excel/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE849C5F-544A-4258-9497-280BFCF0067F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F6B8AF-701E-4B63-9D9B-83D856E8CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="1830" windowWidth="29040" windowHeight="15720" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="9855" yWindow="5265" windowWidth="18090" windowHeight="7770" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -471,7 +471,7 @@
   <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="I5" sqref="I5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -605,7 +605,7 @@
         <v>7</v>
       </c>
       <c r="I4">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="J4">
         <v>3</v>

</xml_diff>

<commit_message>
Feat : Enemy 2종 생성
</commit_message>
<xml_diff>
--- a/Assets/Excel/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77F6B8AF-701E-4B63-9D9B-83D856E8CBF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03FCE923-34C0-4BF3-BF01-D7373D96E13A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9855" yWindow="5265" windowWidth="18090" windowHeight="7770" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,41 +50,40 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>maxHealth</t>
+  </si>
+  <si>
+    <t>attackRange</t>
+  </si>
+  <si>
+    <t>meleeAtk</t>
+  </si>
+  <si>
+    <t>magicAtk</t>
+  </si>
+  <si>
+    <t>def</t>
+  </si>
+  <si>
+    <t>attackSpeed</t>
+  </si>
+  <si>
+    <t>moveSpeed</t>
+  </si>
+  <si>
     <t>Normal</t>
-    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Slime</t>
   </si>
   <si>
     <t>Elite</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>Boss</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Type1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>maxHealth</t>
-  </si>
-  <si>
-    <t>attackRange</t>
-  </si>
-  <si>
-    <t>meleeAtk</t>
-  </si>
-  <si>
-    <t>magicAtk</t>
-  </si>
-  <si>
-    <t>def</t>
-  </si>
-  <si>
-    <t>attackSpeed</t>
-  </si>
-  <si>
-    <t>moveSpeed</t>
+  </si>
+  <si>
+    <t>TurtleShell</t>
   </si>
 </sst>
 </file>
@@ -468,14 +467,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7081A750-B47F-4730-9C09-CC20B4585EF3}">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:J5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="I6" sqref="I6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
@@ -494,25 +495,25 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
       </c>
-      <c r="E1" t="s">
+      <c r="I1" t="s">
         <v>8</v>
       </c>
-      <c r="F1" t="s">
+      <c r="J1" t="s">
         <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>10</v>
-      </c>
-      <c r="H1" t="s">
-        <v>11</v>
-      </c>
-      <c r="I1" t="s">
-        <v>12</v>
-      </c>
-      <c r="J1" t="s">
-        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -520,16 +521,16 @@
         <v>10101</v>
       </c>
       <c r="B2" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="D2">
         <v>30</v>
       </c>
       <c r="E2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -541,10 +542,10 @@
         <v>3</v>
       </c>
       <c r="I2">
-        <v>0.7</v>
+        <v>0.4</v>
       </c>
       <c r="J2">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -552,16 +553,16 @@
         <v>10102</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>50</v>
       </c>
       <c r="E3">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -573,7 +574,7 @@
         <v>5</v>
       </c>
       <c r="I3">
-        <v>0.7</v>
+        <v>0.5</v>
       </c>
       <c r="J3">
         <v>3</v>
@@ -584,16 +585,16 @@
         <v>10103</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="D4">
         <v>700</v>
       </c>
       <c r="E4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F4">
         <v>7</v>
@@ -605,10 +606,42 @@
         <v>7</v>
       </c>
       <c r="I4">
-        <v>0.8</v>
+        <v>0.6</v>
       </c>
       <c r="J4">
         <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>10201</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>30</v>
+      </c>
+      <c r="E5">
+        <v>2</v>
+      </c>
+      <c r="F5">
+        <v>3</v>
+      </c>
+      <c r="G5">
+        <v>0</v>
+      </c>
+      <c r="H5">
+        <v>3</v>
+      </c>
+      <c r="I5">
+        <v>0.4</v>
+      </c>
+      <c r="J5">
+        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat : Enemy 공격판정 구현
데미지 처리는 아직 미구현
</commit_message>
<xml_diff>
--- a/Assets/Excel/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/EnemyDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACB123B4-6444-4046-9F3A-95AFB1C37C7F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3890903A-038D-4E08-9E27-8F46FADD88D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -84,13 +84,17 @@
   </si>
   <si>
     <t>TurtleShell</t>
+  </si>
+  <si>
+    <t>Player Radius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -106,13 +110,28 @@
       <charset val="129"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -129,9 +148,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -467,56 +492,60 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7081A750-B47F-4730-9C09-CC20B4585EF3}">
-  <dimension ref="A1:J5"/>
+  <dimension ref="A1:O15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="O15" sqref="O15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.25" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="4.25" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:15" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10101</v>
       </c>
@@ -530,7 +559,7 @@
         <v>20</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="F2">
         <v>3</v>
@@ -548,7 +577,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10102</v>
       </c>
@@ -562,7 +591,7 @@
         <v>50</v>
       </c>
       <c r="E3">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="F3">
         <v>5</v>
@@ -580,7 +609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>10103</v>
       </c>
@@ -594,7 +623,7 @@
         <v>700</v>
       </c>
       <c r="E4">
-        <v>2</v>
+        <v>1.6</v>
       </c>
       <c r="F4">
         <v>7</v>
@@ -612,7 +641,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>10201</v>
       </c>
@@ -626,7 +655,7 @@
         <v>20</v>
       </c>
       <c r="E5">
-        <v>2</v>
+        <v>1.7</v>
       </c>
       <c r="F5">
         <v>3</v>
@@ -642,6 +671,16 @@
       </c>
       <c r="J5">
         <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="O15">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Feat : Enemy 피격/사망 구현
</commit_message>
<xml_diff>
--- a/Assets/Excel/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05625FA1-DFAC-4BE0-9581-F402D0B25445}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A08ABFB2-35CE-4E56-A8F9-B0D74C6E5FD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6960" yWindow="2625" windowWidth="21690" windowHeight="12015" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+  <si>
+    <t>Normal</t>
+  </si>
+  <si>
+    <t>Slime</t>
+  </si>
+  <si>
+    <t>Elite</t>
+  </si>
+  <si>
+    <t>Boss</t>
+  </si>
+  <si>
+    <t>TurtleShell</t>
+  </si>
+  <si>
+    <t>Player Radius</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Small</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Medium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -50,43 +77,35 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>size</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackRange</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>meleeAtk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>magicAtk</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>def</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>attackSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>moveSpeed</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>maxHealth</t>
-  </si>
-  <si>
-    <t>attackRange</t>
-  </si>
-  <si>
-    <t>meleeAtk</t>
-  </si>
-  <si>
-    <t>magicAtk</t>
-  </si>
-  <si>
-    <t>def</t>
-  </si>
-  <si>
-    <t>attackSpeed</t>
-  </si>
-  <si>
-    <t>moveSpeed</t>
-  </si>
-  <si>
-    <t>Normal</t>
-  </si>
-  <si>
-    <t>Slime</t>
-  </si>
-  <si>
-    <t>Elite</t>
-  </si>
-  <si>
-    <t>Boss</t>
-  </si>
-  <si>
-    <t>TurtleShell</t>
-  </si>
-  <si>
-    <t>Player Radius</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -94,7 +113,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,6 +133,21 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="맑은 고딕"/>
+      <family val="3"/>
+      <charset val="129"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <name val="맑은 고딕"/>
       <family val="3"/>
       <charset val="129"/>
@@ -148,7 +182,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -157,6 +191,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,230 +532,286 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7081A750-B47F-4730-9C09-CC20B4585EF3}">
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:M7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I7" sqref="I7"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="12.625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="5.375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.375" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.75" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.25" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="5.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.875" style="3" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="15.375" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9" style="3"/>
+    <col min="13" max="13" width="13.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="3"/>
+    <col min="15" max="15" width="13.125" style="3" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" s="2" customFormat="1" ht="20.25">
       <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13">
+      <c r="A2" s="3">
+        <v>30000000</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="D2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="3">
+        <v>20</v>
+      </c>
+      <c r="F2" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G2" s="3">
+        <v>3</v>
+      </c>
+      <c r="H2" s="3">
+        <v>0</v>
+      </c>
+      <c r="I2" s="3">
+        <v>3</v>
+      </c>
+      <c r="J2" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K2" s="3">
+        <v>2</v>
+      </c>
+      <c r="M2" s="3">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13">
+      <c r="A3" s="3">
+        <v>30010001</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="D3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="3">
+        <v>50</v>
+      </c>
+      <c r="F3" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G3" s="3">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3">
+        <v>0</v>
+      </c>
+      <c r="I3" s="3">
+        <v>5</v>
+      </c>
+      <c r="J3" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K3" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13">
+      <c r="A4" s="3">
+        <v>30020001</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E4" s="3">
+        <v>700</v>
+      </c>
+      <c r="F4" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G4" s="3">
+        <v>7</v>
+      </c>
+      <c r="H4" s="3">
+        <v>0</v>
+      </c>
+      <c r="I4" s="3">
+        <v>7</v>
+      </c>
+      <c r="J4" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K4" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13">
+      <c r="A5" s="3">
+        <v>30100000</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="E5" s="3">
+        <v>20</v>
+      </c>
+      <c r="F5" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="G5" s="3">
+        <v>3</v>
+      </c>
+      <c r="H5" s="3">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>3</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K5" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13">
+      <c r="A6" s="3">
+        <v>30110001</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>9</v>
+      <c r="E6" s="3">
+        <v>50</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="G6" s="3">
+        <v>3</v>
+      </c>
+      <c r="H6" s="3">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>3</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K6" s="3">
+        <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>10101</v>
-      </c>
-      <c r="B2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
-        <v>20</v>
-      </c>
-      <c r="E2">
-        <v>1.6</v>
-      </c>
-      <c r="F2">
-        <v>3</v>
-      </c>
-      <c r="G2">
+    <row r="7" spans="1:13">
+      <c r="A7" s="3">
+        <v>30120001</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="E7" s="3">
+        <v>700</v>
+      </c>
+      <c r="F7" s="3">
+        <v>1.7</v>
+      </c>
+      <c r="G7" s="3">
+        <v>7</v>
+      </c>
+      <c r="H7" s="3">
         <v>0</v>
       </c>
-      <c r="H2">
-        <v>3</v>
-      </c>
-      <c r="I2">
+      <c r="I7" s="3">
+        <v>7</v>
+      </c>
+      <c r="J7" s="3">
         <v>0.5</v>
       </c>
-      <c r="J2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A3">
-        <v>10102</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D3">
-        <v>50</v>
-      </c>
-      <c r="E3">
-        <v>1.6</v>
-      </c>
-      <c r="F3">
-        <v>5</v>
-      </c>
-      <c r="G3">
-        <v>0</v>
-      </c>
-      <c r="H3">
-        <v>5</v>
-      </c>
-      <c r="I3">
-        <v>0.5</v>
-      </c>
-      <c r="J3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4">
-        <v>10103</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>700</v>
-      </c>
-      <c r="E4">
-        <v>1.6</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <v>0.5</v>
-      </c>
-      <c r="J4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A5">
-        <v>10201</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>20</v>
-      </c>
-      <c r="E5">
-        <v>1.7</v>
-      </c>
-      <c r="F5">
-        <v>3</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-      <c r="H5">
-        <v>3</v>
-      </c>
-      <c r="I5">
-        <v>0.5</v>
-      </c>
-      <c r="J5">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A6">
-        <v>10202</v>
-      </c>
-      <c r="B6" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6">
-        <v>50</v>
-      </c>
-      <c r="E6">
-        <v>1.7</v>
-      </c>
-      <c r="F6">
-        <v>3</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6">
-        <v>3</v>
-      </c>
-      <c r="I6">
-        <v>0.5</v>
-      </c>
-      <c r="J6">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O14" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="O15">
-        <v>0.5</v>
+      <c r="K7" s="3">
+        <v>3</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K7">
+    <sortCondition ref="A1:A7"/>
+  </sortState>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Feat : EnemyDB 데이터 추가 및 Enemy 설정
Enemy DB에 다른 종족들 ID별로 추가

Enemy별로 AgentType 설정

콜라이더는 아직 CharacterController를 쓸지말지안정해서 미뤄둠
</commit_message>
<xml_diff>
--- a/Assets/Excel/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA97509-AB37-4F2A-9504-078C5674EF18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB00AAAD-2C36-45B2-ADBF-664A06AB11AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="-27000" yWindow="1950" windowWidth="27105" windowHeight="15585" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
   <si>
     <t>Normal</t>
   </si>
@@ -107,6 +107,37 @@
   <si>
     <t>maxHealth</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Spider</t>
+  </si>
+  <si>
+    <t>Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Skeleton</t>
+  </si>
+  <si>
+    <t>Orc</t>
+  </si>
+  <si>
+    <t>Golem</t>
+  </si>
+  <si>
+    <t>Bat</t>
+  </si>
+  <si>
+    <t>Dragon</t>
+  </si>
+  <si>
+    <t>Medium</t>
+  </si>
+  <si>
+    <t>Small</t>
+  </si>
+  <si>
+    <t>MonsterPlant</t>
   </si>
 </sst>
 </file>
@@ -532,15 +563,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7081A750-B47F-4730-9C09-CC20B4585EF3}">
-  <dimension ref="A1:M7"/>
+  <dimension ref="A1:M14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S6" sqref="S6"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="1" max="2" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.5" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.125" style="3" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="7.75" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="14.25" style="3" bestFit="1" customWidth="1"/>
@@ -808,6 +840,251 @@
         <v>3</v>
       </c>
     </row>
+    <row r="8" spans="1:13">
+      <c r="A8" s="3">
+        <v>30200000</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E8" s="3">
+        <v>20</v>
+      </c>
+      <c r="F8" s="3">
+        <v>1.6</v>
+      </c>
+      <c r="G8" s="3">
+        <v>3</v>
+      </c>
+      <c r="H8" s="3">
+        <v>0</v>
+      </c>
+      <c r="I8" s="3">
+        <v>3</v>
+      </c>
+      <c r="J8" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K8" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13">
+      <c r="A9" s="3">
+        <v>30300000</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E9" s="3">
+        <v>20</v>
+      </c>
+      <c r="F9" s="3">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="G9" s="3">
+        <v>3</v>
+      </c>
+      <c r="H9" s="3">
+        <v>0</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3</v>
+      </c>
+      <c r="J9" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K9" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13">
+      <c r="A10" s="3">
+        <v>30400001</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E10" s="3">
+        <v>20</v>
+      </c>
+      <c r="F10" s="3">
+        <v>3</v>
+      </c>
+      <c r="G10" s="3">
+        <v>3</v>
+      </c>
+      <c r="H10" s="3">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>3</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K10" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13">
+      <c r="A11" s="3">
+        <v>30700001</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E11" s="3">
+        <v>20</v>
+      </c>
+      <c r="F11" s="3">
+        <v>2.5</v>
+      </c>
+      <c r="G11" s="3">
+        <v>3</v>
+      </c>
+      <c r="H11" s="3">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>3</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K11" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="3">
+        <v>30600000</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="3">
+        <v>20</v>
+      </c>
+      <c r="F12" s="3">
+        <v>2</v>
+      </c>
+      <c r="G12" s="3">
+        <v>3</v>
+      </c>
+      <c r="H12" s="3">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>3</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K12" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13">
+      <c r="A13" s="3">
+        <v>30700000</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="3">
+        <v>20</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>3</v>
+      </c>
+      <c r="H13" s="3">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>3</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K13" s="3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13">
+      <c r="A14" s="3">
+        <v>30800000</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E14" s="3">
+        <v>20</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>3</v>
+      </c>
+      <c r="H14" s="3">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0.5</v>
+      </c>
+      <c r="K14" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K7">
     <sortCondition ref="A1:A7"/>

</xml_diff>

<commit_message>
Feat : EvilMage 데이터 구현
</commit_message>
<xml_diff>
--- a/Assets/Excel/EnemyDB_Sheet.xlsx
+++ b/Assets/Excel/EnemyDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rlqja\Unity Project\Sisyphus\Assets\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB00AAAD-2C36-45B2-ADBF-664A06AB11AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D626326-27AC-4ABD-9570-348B6015F74F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-27000" yWindow="1950" windowWidth="27105" windowHeight="15585" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
+    <workbookView xWindow="-27660" yWindow="2085" windowWidth="27105" windowHeight="15585" xr2:uid="{FB33F838-1C05-4B66-BC08-EB445EFDF3F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Entities" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="30">
   <si>
     <t>Normal</t>
   </si>
@@ -138,6 +138,9 @@
   </si>
   <si>
     <t>MonsterPlant</t>
+  </si>
+  <si>
+    <t>EvilMage</t>
   </si>
 </sst>
 </file>
@@ -563,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7081A750-B47F-4730-9C09-CC20B4585EF3}">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:M15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5"/>
@@ -1085,6 +1088,41 @@
         <v>2</v>
       </c>
     </row>
+    <row r="15" spans="1:13">
+      <c r="A15" s="3">
+        <v>30900000</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E15" s="3">
+        <v>20</v>
+      </c>
+      <c r="F15" s="3">
+        <v>7</v>
+      </c>
+      <c r="G15" s="3">
+        <v>0</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3</v>
+      </c>
+      <c r="I15" s="3">
+        <v>3</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0.3</v>
+      </c>
+      <c r="K15" s="3">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:K7">
     <sortCondition ref="A1:A7"/>

</xml_diff>